<commit_message>
reading data from excel and credentials from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\dsalgo_ninjalinos-BDD\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61E8C82B-2E41-4B79-84E2-9A3BFA07F7ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D110470-DEC2-4FE8-980B-897F62ED5092}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{0115BC9B-6D92-47C7-9547-34A77FBE44D5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{0115BC9B-6D92-47C7-9547-34A77FBE44D5}"/>
   </bookViews>
   <sheets>
     <sheet name="TextEditor" sheetId="1" r:id="rId1"/>
+    <sheet name="credentials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Valid Code</t>
   </si>
@@ -52,19 +53,44 @@
   </si>
   <si>
     <t>Hello World</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>ninjalinos@work.com</t>
+  </si>
+  <si>
+    <t>sdet218920@</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,8 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C8A219-A3E7-414E-8157-F48EFA2DEC9B}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -452,4 +480,40 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B861D3D5-735F-4741-95FD-F5379CAA3E3D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ran both modules succesfully with excel reader using Login Page
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\dsalgo_ninjalinos-BDD\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpitgupta/git/dsalgo_ninjalinos-BDD/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D110470-DEC2-4FE8-980B-897F62ED5092}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FFE877-149B-094B-9987-EC8F73D2884D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{0115BC9B-6D92-47C7-9547-34A77FBE44D5}"/>
+    <workbookView xWindow="6100" yWindow="8440" windowWidth="15340" windowHeight="8200" activeTab="1" xr2:uid="{0115BC9B-6D92-47C7-9547-34A77FBE44D5}"/>
   </bookViews>
   <sheets>
-    <sheet name="TextEditor" sheetId="1" r:id="rId1"/>
+    <sheet name="textEditor" sheetId="1" r:id="rId1"/>
     <sheet name="credentials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
@@ -135,9 +135,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +175,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -281,7 +281,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -423,7 +423,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -437,16 +437,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -490,13 +490,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -504,7 +504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
reading data from excel for practice questions
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpitgupta/git/dsalgo_ninjalinos-BDD/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FFE877-149B-094B-9987-EC8F73D2884D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D20A1E-FAB6-BC48-B67D-4495BBF7613F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="8440" windowWidth="15340" windowHeight="8200" activeTab="1" xr2:uid="{0115BC9B-6D92-47C7-9547-34A77FBE44D5}"/>
+    <workbookView xWindow="4680" yWindow="2980" windowWidth="22980" windowHeight="10640" activeTab="1" xr2:uid="{0115BC9B-6D92-47C7-9547-34A77FBE44D5}"/>
   </bookViews>
   <sheets>
     <sheet name="textEditor" sheetId="1" r:id="rId1"/>
-    <sheet name="credentials" sheetId="2" r:id="rId2"/>
+    <sheet name="practiceQ" sheetId="3" r:id="rId2"/>
+    <sheet name="credentials" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Valid Code</t>
   </si>
@@ -65,6 +66,18 @@
   </si>
   <si>
     <t>sdet218920@</t>
+  </si>
+  <si>
+    <t>Valid code</t>
+  </si>
+  <si>
+    <t>Invalid Code</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>print 'hello'</t>
   </si>
 </sst>
 </file>
@@ -113,10 +126,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +503,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71214FDB-D257-C046-BAFA-1DA8504A6E6F}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="69" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B861D3D5-735F-4741-95FD-F5379CAA3E3D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reported bug for practice question page in LL
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpitgupta/git/dsalgo_ninjalinos-BDD/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D20A1E-FAB6-BC48-B67D-4495BBF7613F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0337DC1B-CB88-C046-BA79-3ADC6C9271A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="2980" windowWidth="22980" windowHeight="10640" activeTab="1" xr2:uid="{0115BC9B-6D92-47C7-9547-34A77FBE44D5}"/>
+    <workbookView xWindow="4680" yWindow="2980" windowWidth="22980" windowHeight="10640" xr2:uid="{0115BC9B-6D92-47C7-9547-34A77FBE44D5}"/>
   </bookViews>
   <sheets>
-    <sheet name="textEditor" sheetId="1" r:id="rId1"/>
-    <sheet name="practiceQ" sheetId="3" r:id="rId2"/>
-    <sheet name="credentials" sheetId="2" r:id="rId3"/>
+    <sheet name="TextEditor" sheetId="1" r:id="rId1"/>
+    <sheet name="Credentials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Valid Code</t>
   </si>
@@ -66,18 +65,6 @@
   </si>
   <si>
     <t>sdet218920@</t>
-  </si>
-  <si>
-    <t>Valid code</t>
-  </si>
-  <si>
-    <t>Invalid Code</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>print 'hello'</t>
   </si>
 </sst>
 </file>
@@ -126,17 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C8A219-A3E7-414E-8157-F48EFA2DEC9B}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -503,43 +483,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71214FDB-D257-C046-BAFA-1DA8504A6E6F}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="69" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B861D3D5-735F-4741-95FD-F5379CAA3E3D}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>